<commit_message>
Added Rest assured code
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Ahilesh\SeleniumAhilesh\SeleniumFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7ED730-411C-4D8E-A11A-B0A253A24E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49BEBEE-12F5-4337-9C66-026D3D13DFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1242E302-FE69-4E04-93EB-CD7785C82CB4}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>